<commit_message>
US-13314 [IMP] PO/Catalogue mismatch: Added 2 columns to the export and fixed the report name when exporting from form view
</commit_message>
<xml_diff>
--- a/bin/addons/purchase/report/line_mismatch.xlsx
+++ b/bin/addons/purchase/report/line_mismatch.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\rha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.123.1\partage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9B033D0-DE5A-46B7-9FAE-1973A8816433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410"/>
   </bookViews>
   <sheets>
     <sheet name="PO Catalogue Mismatch" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Product Code</t>
   </si>
@@ -124,9 +123,6 @@
     <t>Catalogue SoQ</t>
   </si>
   <si>
-    <t>PO Price</t>
-  </si>
-  <si>
     <t>PO Quantity</t>
   </si>
   <si>
@@ -143,6 +139,15 @@
   </si>
   <si>
     <t>Catalogue To date: XX/XX/XXXX</t>
+  </si>
+  <si>
+    <t>PO Unit Price</t>
+  </si>
+  <si>
+    <t>PO Subtotal</t>
+  </si>
+  <si>
+    <t>Catalogue Subtotal</t>
   </si>
 </sst>
 </file>
@@ -672,48 +677,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1025,30 +1030,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="11.109375" customWidth="1"/>
-    <col min="12" max="12" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="20" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="22" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1056,7 +1061,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1064,7 +1069,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1072,23 +1077,23 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1096,7 +1101,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1107,61 +1112,67 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1180,29 +1191,27 @@
       <c r="F11" s="2">
         <v>18956.87</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="2">
+        <v>18956.87</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>45301</v>
       </c>
-      <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="P11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>19</v>
@@ -1211,18 +1220,24 @@
         <v>19</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="U11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
US-14491 [IMP] PO Catalogue tab: Added % deviation at header and line level, price is bold if higher than the catalogue, fixed a column name, and added deviation to the mismatch report
</commit_message>
<xml_diff>
--- a/bin/addons/purchase/report/line_mismatch.xlsx
+++ b/bin/addons/purchase/report/line_mismatch.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.123.1\partage1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.122.1\partage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Product Code</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Catalogue Subtotal</t>
+  </si>
+  <si>
+    <t>% Price Deviation</t>
   </si>
 </sst>
 </file>
@@ -1030,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,17 +1046,17 @@
     <col min="4" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.140625" customWidth="1"/>
-    <col min="14" max="14" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="22" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="23" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1139,40 +1142,43 @@
         <v>42</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1204,17 +1210,15 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
-      <c r="N11" s="2" t="s">
+      <c r="N11" s="3"/>
+      <c r="O11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="R11" s="2" t="s">
         <v>19</v>
@@ -1226,16 +1230,19 @@
         <v>19</v>
       </c>
       <c r="U11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V11" s="2" t="s">
+      <c r="W11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="X11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
US-14491 [FIX] PO Catalogue tab: fixed columns order and header % deviation. PO Catalogue mismatch report: Fixed columns order, added adherence summary to the header and changed header style
</commit_message>
<xml_diff>
--- a/bin/addons/purchase/report/line_mismatch.xlsx
+++ b/bin/addons/purchase/report/line_mismatch.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Product Code</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Catalogue Price</t>
   </si>
   <si>
-    <t>Catalogue SoQ</t>
-  </si>
-  <si>
     <t>PO Quantity</t>
   </si>
   <si>
@@ -147,10 +144,22 @@
     <t>PO Subtotal</t>
   </si>
   <si>
-    <t>Catalogue Subtotal</t>
-  </si>
-  <si>
     <t>% Price Deviation</t>
+  </si>
+  <si>
+    <t>Catalogue adherence summary</t>
+  </si>
+  <si>
+    <t>PO lines adherence: X% PO Lines Mismatch: X% of which Not in catalogue: X%</t>
+  </si>
+  <si>
+    <t>% deviation of PO subtotal vs theoretical catalogue subtotal (for catalogue lines): X%</t>
+  </si>
+  <si>
+    <t>Catalogue Unit Price</t>
+  </si>
+  <si>
+    <t>Cataogue Subtotal</t>
   </si>
 </sst>
 </file>
@@ -488,7 +497,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -618,6 +627,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -663,7 +701,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -674,8 +712,28 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1033,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X13"/>
+  <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,210 +1102,291 @@
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="11.140625" customWidth="1"/>
+    <col min="6" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.140625" customWidth="1"/>
     <col min="15" max="15" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="23" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="A1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="5">
+      <c r="B7" s="4"/>
+      <c r="C7" s="10">
         <v>45314</v>
       </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
     </row>
-    <row r="10" spans="1:24" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="13" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O10" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="T13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="U13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="V13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="W13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="X13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="14" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>3</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F14" s="2">
         <v>18956.87</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G14" s="2">
         <v>18956.87</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H14" s="2">
+        <v>18956.87</v>
+      </c>
+      <c r="I14" s="2">
+        <v>18956.87</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="3">
+      <c r="K14" s="3"/>
+      <c r="L14" s="3">
         <v>45301</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="2" t="s">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="R14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S11" s="2" t="s">
+      <c r="S14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T11" s="2" t="s">
+      <c r="T14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="U14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V11" s="2" t="s">
+      <c r="V14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="W14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="X11" s="2" t="s">
+      <c r="X14" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>37</v>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>